<commit_message>
latest timing for omp
git-svn-id: svn://136.177.114.72/svn_GW/phast3/trunk@9578 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/src/phast/yeti.xlsx
+++ b/src/phast/yeti.xlsx
@@ -355,10 +355,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$B$19</c:f>
+              <c:f>Sheet1!$B$14:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -376,16 +376,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$14:$M$19</c:f>
+              <c:f>Sheet1!$M$14:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -403,6 +409,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.192155854657702</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6429873182802353</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3094867230381249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -509,11 +521,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1853046576"/>
-        <c:axId val="1853047184"/>
+        <c:axId val="-476038768"/>
+        <c:axId val="-476038224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1853046576"/>
+        <c:axId val="-476038768"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -614,12 +626,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853047184"/>
+        <c:crossAx val="-476038224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1853047184"/>
+        <c:axId val="-476038224"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -733,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853046576"/>
+        <c:crossAx val="-476038768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -891,8 +903,88 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Easy</c:v>
           </c:tx>
@@ -910,35 +1002,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
+              <c:f>Sheet1!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
@@ -946,36 +1032,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$11</c:f>
+              <c:f>Sheet1!$N$5:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9396612348687736</c:v>
+                  <c:v>1.9650278806165029</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6771851094448227</c:v>
+                  <c:v>3.5930308071967993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.2257712622469237</c:v>
+                  <c:v>6.5194512246443903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.212239382000583</c:v>
+                  <c:v>8.9726156459958322</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.973228965014165</c:v>
+                  <c:v>13.781183280352995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.993968646227508</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50.675961949043987</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50.158362487966379</c:v>
+                  <c:v>13.640423583554441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,7 +1064,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Medium</c:v>
           </c:tx>
@@ -1002,35 +1082,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$22:$B$30</c:f>
+              <c:f>Sheet1!$B$26:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
@@ -1038,36 +1112,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$22:$M$30</c:f>
+              <c:f>Sheet1!$N$26:$N$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9147864141712945</c:v>
+                  <c:v>1.8314352724510956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5691782919086168</c:v>
+                  <c:v>3.210475032551241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5367190174681928</c:v>
+                  <c:v>5.4475729519038305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.458757792896499</c:v>
+                  <c:v>8.4998424779811597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.443359123523695</c:v>
+                  <c:v>12.180760573701841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.337453257053102</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43.475306218592955</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42.183299156260112</c:v>
+                  <c:v>11.81877051417978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,7 +1144,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Hard</c:v>
           </c:tx>
@@ -1094,164 +1162,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$41</c:f>
+              <c:f>Sheet1!$B$37:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>196</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$33:$M$41</c:f>
+              <c:f>Sheet1!$N$37:$N$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9396612348687736</c:v>
+                  <c:v>1.8629820144077587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6771851094448227</c:v>
+                  <c:v>3.3375761511239097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.2257712622469237</c:v>
+                  <c:v>5.7368456370209451</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.212239382000583</c:v>
+                  <c:v>9.6499884303024484</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.973228965014165</c:v>
+                  <c:v>15.79272948384415</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0187193943874737</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50.675961949043987</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50.158362487966379</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Ideal</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>192</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>192</c:v>
+                  <c:v>17.841318562832598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,15 +1230,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1860447824"/>
-        <c:axId val="1860455120"/>
+        <c:axId val="-516146240"/>
+        <c:axId val="-516145152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1860447824"/>
+        <c:axId val="-516146240"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="256"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1371,12 +1336,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860455120"/>
+        <c:crossAx val="-516145152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1860455120"/>
+        <c:axId val="-516145152"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1453,7 +1418,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1490,7 +1455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860447824"/>
+        <c:crossAx val="-516146240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2687,16 +2652,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2717,16 +2682,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3013,17 +2978,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="5" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.77734375" customWidth="1"/>
+    <col min="10" max="12" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -3167,6 +3134,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>B5/$B$5</f>
+        <v>1</v>
+      </c>
       <c r="B5">
         <v>4</v>
       </c>
@@ -3206,11 +3177,19 @@
         <v>3.724206651048164</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M11" si="5">$J$3/J5</f>
+        <f t="shared" ref="M5:M10" si="5">$J$3/J5</f>
         <v>3.6771851094448227</v>
+      </c>
+      <c r="N5" s="2">
+        <f>$J$5/J5</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" ref="A6:A11" si="6">B6/$B$5</f>
+        <v>2</v>
+      </c>
       <c r="B6">
         <v>8</v>
       </c>
@@ -3253,8 +3232,16 @@
         <f t="shared" si="5"/>
         <v>7.2257712622469237</v>
       </c>
+      <c r="N6" s="2">
+        <f t="shared" ref="N6:N11" si="7">$J$5/J6</f>
+        <v>1.9650278806165029</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
       <c r="B7">
         <v>16</v>
       </c>
@@ -3297,8 +3284,16 @@
         <f t="shared" si="5"/>
         <v>13.212239382000583</v>
       </c>
+      <c r="N7" s="2">
+        <f t="shared" si="7"/>
+        <v>3.5930308071967993</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
       <c r="B8">
         <v>32</v>
       </c>
@@ -3341,8 +3336,16 @@
         <f t="shared" si="5"/>
         <v>23.973228965014165</v>
       </c>
+      <c r="N8" s="2">
+        <f t="shared" si="7"/>
+        <v>6.5194512246443903</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
       <c r="B9">
         <v>64</v>
       </c>
@@ -3385,8 +3388,16 @@
         <f t="shared" si="5"/>
         <v>32.993968646227508</v>
       </c>
+      <c r="N9" s="2">
+        <f t="shared" si="7"/>
+        <v>8.9726156459958322</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
       <c r="B10">
         <v>128</v>
       </c>
@@ -3429,8 +3440,16 @@
         <f t="shared" si="5"/>
         <v>50.675961949043987</v>
       </c>
+      <c r="N10" s="2">
+        <f t="shared" si="7"/>
+        <v>13.781183280352995</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
       <c r="B11">
         <v>192</v>
       </c>
@@ -3444,7 +3463,7 @@
         <v>587.71</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" ref="F11" si="6">E11+D11</f>
+        <f t="shared" ref="F11" si="8">E11+D11</f>
         <v>635.92000000000007</v>
       </c>
       <c r="G11" s="2">
@@ -3462,7 +3481,7 @@
         <v>851.78</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" ref="K11" si="7">SUM(C11:H11)</f>
+        <f t="shared" ref="K11" si="9">SUM(C11:H11)</f>
         <v>2125.3000000000002</v>
       </c>
       <c r="L11" s="2">
@@ -3472,6 +3491,10 @@
       <c r="M11" s="2">
         <f>$J$3/J11</f>
         <v>50.158362487966379</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="7"/>
+        <v>13.640423583554441</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -3539,7 +3562,7 @@
         <v>1108</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" ref="I14:I19" si="8">G14</f>
+        <f t="shared" ref="I14:I21" si="10">G14</f>
         <v>41304.5</v>
       </c>
       <c r="J14" s="2">
@@ -3573,7 +3596,7 @@
         <v>17.63</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" ref="F15:F19" si="9">E15+D15</f>
+        <f t="shared" ref="F15:F21" si="11">E15+D15</f>
         <v>2417.2600000000002</v>
       </c>
       <c r="G15" s="2">
@@ -3583,7 +3606,7 @@
         <v>845.38</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21521.13</v>
       </c>
       <c r="J15" s="2">
@@ -3599,7 +3622,7 @@
         <v>1.9337827521138529</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ref="M15:M18" si="10">$J$3/J15</f>
+        <f t="shared" ref="M15:M18" si="12">$J$3/J15</f>
         <v>1.9101723961404795</v>
       </c>
       <c r="P15" s="3"/>
@@ -3618,7 +3641,7 @@
         <v>19.63</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1553.0100000000002</v>
       </c>
       <c r="G16" s="2">
@@ -3628,28 +3651,28 @@
         <v>758.5</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10877.25</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" ref="J16:J19" si="11">H16+G16</f>
+        <f t="shared" ref="J16:J21" si="13">H16+G16</f>
         <v>11635.75</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" ref="K16:K17" si="12">SUM(C16:H16)</f>
+        <f t="shared" ref="K16:K17" si="14">SUM(C16:H16)</f>
         <v>14743.27</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" ref="L16:L17" si="13">$I$3/I16</f>
+        <f t="shared" ref="L16:L17" si="15">$I$3/I16</f>
         <v>3.8260764439541246</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.6717779257890553</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>8</v>
       </c>
@@ -3663,7 +3686,7 @@
         <v>67.63</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2044.0100000000002</v>
       </c>
       <c r="G17" s="2">
@@ -3673,27 +3696,27 @@
         <v>961.88</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5946.63</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6908.51</v>
       </c>
       <c r="K17" s="2">
+        <f t="shared" si="14"/>
+        <v>11005.28</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="15"/>
+        <v>6.9984495420095083</v>
+      </c>
+      <c r="M17" s="2">
         <f t="shared" si="12"/>
-        <v>11005.28</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="13"/>
-        <v>6.9984495420095083</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="10"/>
         <v>6.1842408855165587</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -3707,7 +3730,7 @@
         <v>33.22</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1459.8500000000001</v>
       </c>
       <c r="G18" s="2">
@@ -3717,11 +3740,11 @@
         <v>1699.91</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3442.97</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5142.88</v>
       </c>
       <c r="K18" s="2">
@@ -3733,11 +3756,11 @@
         <v>12.087584265909957</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8.3073861338394046</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
@@ -3751,7 +3774,7 @@
         <v>33.380000000000003</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6571.76</v>
       </c>
       <c r="G19" s="2">
@@ -3761,11 +3784,11 @@
         <v>8057.44</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>11432</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19489.439999999999</v>
       </c>
       <c r="K19" s="2">
@@ -3777,960 +3800,1088 @@
         <v>3.6404120013995804</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" ref="M19" si="14">$J$3/J19</f>
+        <f t="shared" ref="M19:M21" si="16">$J$3/J19</f>
         <v>2.192155854657702</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6687.75</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43.13</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="11"/>
+        <v>6730.88</v>
+      </c>
+      <c r="G20" s="2">
+        <v>7414.25</v>
+      </c>
+      <c r="H20" s="2">
+        <v>8750.75</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="10"/>
+        <v>7414.25</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="13"/>
+        <v>16165</v>
+      </c>
+      <c r="K20" s="2">
+        <f>SUM(C20:H20)</f>
+        <v>29630.760000000002</v>
+      </c>
+      <c r="L20" s="2">
+        <f>$I$3/I20</f>
+        <v>5.6131355160670333</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="16"/>
+        <v>2.6429873182802353</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2">
+        <v>10.63</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10673.88</v>
+      </c>
+      <c r="E21" s="2">
+        <v>105.63</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="11"/>
+        <v>10779.509999999998</v>
+      </c>
+      <c r="G21" s="2">
+        <v>11745.56</v>
+      </c>
+      <c r="H21" s="2">
+        <v>20880.88</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="10"/>
+        <v>11745.56</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="13"/>
+        <v>32626.440000000002</v>
+      </c>
+      <c r="K21" s="2">
+        <f>SUM(C21:H21)</f>
+        <v>54196.09</v>
+      </c>
+      <c r="L21" s="2">
+        <f>$I$3/I21</f>
+        <v>3.5432273982679416</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="16"/>
+        <v>1.3094867230381249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B22">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C24" s="2">
         <v>3.78</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D24" s="2">
         <v>2630.7</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E24" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="F22" s="2">
-        <f>E22+D22</f>
+      <c r="F24" s="2">
+        <f>E24+D24</f>
         <v>2650.6</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G24" s="2">
         <v>65326.559999999998</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H24" s="2">
         <v>1117.6199999999999</v>
       </c>
-      <c r="I22" s="2">
-        <f>G22</f>
+      <c r="I24" s="2">
+        <f>G24</f>
         <v>65326.559999999998</v>
       </c>
-      <c r="J22" s="2">
-        <f>H22+G22</f>
+      <c r="J24" s="2">
+        <f>H24+G24</f>
         <v>66444.179999999993</v>
       </c>
-      <c r="K22" s="2">
-        <f>H22+G22+E22+D22+C22</f>
+      <c r="K24" s="2">
+        <f>H24+G24+E24+D24+C24</f>
         <v>69098.559999999983</v>
       </c>
-      <c r="L22" s="2">
-        <f>$I$22/I22</f>
+      <c r="L24" s="2">
+        <f>$I$24/I24</f>
         <v>1</v>
       </c>
-      <c r="M22" s="2">
-        <f>$J$22/J22</f>
+      <c r="M24" s="2">
+        <f>$J$24/J24</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B23">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C25" s="2">
         <v>4.49</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D25" s="2">
         <v>1316.61</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E25" s="2">
         <v>349.21</v>
       </c>
-      <c r="F23" s="2">
-        <f t="shared" ref="F23:F30" si="15">E23+D23</f>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F32" si="17">E25+D25</f>
         <v>1665.82</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G25" s="2">
         <v>34024.86</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H25" s="2">
         <v>675.71</v>
       </c>
-      <c r="I23" s="2">
-        <f>G23</f>
+      <c r="I25" s="2">
+        <f>G25</f>
         <v>34024.86</v>
       </c>
-      <c r="J23" s="2">
-        <f>H23+G23</f>
+      <c r="J25" s="2">
+        <f>H25+G25</f>
         <v>34700.57</v>
       </c>
-      <c r="K23" s="2">
-        <f t="shared" ref="K23:K29" si="16">H23+G23+E23+D23+C23</f>
+      <c r="K25" s="2">
+        <f t="shared" ref="K25:K31" si="18">H25+G25+E25+D25+C25</f>
         <v>36370.879999999997</v>
       </c>
-      <c r="L23" s="2">
-        <f t="shared" ref="L23:L30" si="17">$I$22/I23</f>
+      <c r="L25" s="2">
+        <f t="shared" ref="L25:L32" si="19">$I$24/I25</f>
         <v>1.9199655781096527</v>
       </c>
-      <c r="M23" s="2">
-        <f t="shared" ref="M23:M30" si="18">$J$22/J23</f>
+      <c r="M25" s="2">
+        <f t="shared" ref="M25:M32" si="20">$J$24/J25</f>
         <v>1.9147864141712945</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B24">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26">
         <v>4</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C26" s="2">
         <v>4.5599999999999996</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D26" s="2">
         <v>553.30999999999995</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E26" s="2">
         <v>476.04</v>
       </c>
-      <c r="F24" s="2">
-        <f t="shared" si="15"/>
+      <c r="F26" s="2">
+        <f t="shared" si="17"/>
         <v>1029.3499999999999</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G26" s="2">
         <v>18121.14</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H26" s="2">
         <v>494.96</v>
       </c>
-      <c r="I24" s="2">
-        <f t="shared" ref="I24:I30" si="19">G24</f>
+      <c r="I26" s="2">
+        <f t="shared" ref="I26:I32" si="21">G26</f>
         <v>18121.14</v>
       </c>
-      <c r="J24" s="2">
-        <f t="shared" ref="J24:J30" si="20">H24+G24</f>
+      <c r="J26" s="2">
+        <f t="shared" ref="J26:J32" si="22">H26+G26</f>
         <v>18616.099999999999</v>
       </c>
-      <c r="K24" s="2">
-        <f t="shared" si="16"/>
+      <c r="K26" s="2">
+        <f t="shared" si="18"/>
         <v>19650.010000000002</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L26" s="2">
+        <f t="shared" si="19"/>
+        <v>3.6049917389303321</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="20"/>
+        <v>3.5691782919086168</v>
+      </c>
+      <c r="N26" s="2">
+        <f>$J$26/J26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4.59</v>
+      </c>
+      <c r="D27" s="2">
+        <v>89.4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>609.38</v>
+      </c>
+      <c r="F27" s="2">
         <f t="shared" si="17"/>
-        <v>3.6049917389303321</v>
-      </c>
-      <c r="M24" s="2">
+        <v>698.78</v>
+      </c>
+      <c r="G27" s="2">
+        <v>9847.83</v>
+      </c>
+      <c r="H27" s="2">
+        <v>316.93</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="21"/>
+        <v>9847.83</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="22"/>
+        <v>10164.76</v>
+      </c>
+      <c r="K27" s="2">
         <f t="shared" si="18"/>
-        <v>3.5691782919086168</v>
+        <v>10868.13</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="19"/>
+        <v>6.633599483337953</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="20"/>
+        <v>6.5367190174681928</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" ref="N27:N32" si="23">$J$26/J27</f>
+        <v>1.8314352724510956</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="D28" s="2">
+        <v>121.17</v>
+      </c>
+      <c r="E28" s="2">
+        <v>610.03</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="17"/>
+        <v>731.19999999999993</v>
+      </c>
+      <c r="G28" s="2">
+        <v>5489.39</v>
+      </c>
+      <c r="H28" s="2">
+        <v>309.16000000000003</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="21"/>
+        <v>5489.39</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="22"/>
+        <v>5798.55</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="18"/>
+        <v>6535.38</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="19"/>
+        <v>11.90051353611239</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="20"/>
+        <v>11.458757792896499</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="23"/>
+        <v>3.210475032551241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3.31</v>
+      </c>
+      <c r="D29" s="2">
+        <v>191.77</v>
+      </c>
+      <c r="E29" s="2">
+        <v>572.22</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="17"/>
+        <v>763.99</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3196.4</v>
+      </c>
+      <c r="H29" s="2">
+        <v>220.92</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="21"/>
+        <v>3196.4</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="22"/>
+        <v>3417.32</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="18"/>
+        <v>4184.6200000000008</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="19"/>
+        <v>20.437542235014391</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="20"/>
+        <v>19.443359123523695</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="23"/>
+        <v>5.4475729519038305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>64</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>356.63</v>
+      </c>
+      <c r="E30" s="2">
+        <v>531.79</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="17"/>
+        <v>888.42</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1917.8</v>
+      </c>
+      <c r="H30" s="2">
+        <v>272.37</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="21"/>
+        <v>1917.8</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="22"/>
+        <v>2190.17</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="18"/>
+        <v>3079.59</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="19"/>
+        <v>34.063280842632182</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="20"/>
+        <v>30.337453257053102</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="23"/>
+        <v>8.4998424779811597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>128</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="D31" s="2">
+        <v>51.01</v>
+      </c>
+      <c r="E31" s="2">
+        <v>549.41999999999996</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="17"/>
+        <v>600.42999999999995</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1210.3800000000001</v>
+      </c>
+      <c r="H31" s="2">
+        <v>317.94</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="21"/>
+        <v>1210.3800000000001</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="22"/>
+        <v>1528.3200000000002</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="18"/>
+        <v>2130.1100000000006</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="19"/>
+        <v>53.971942695682344</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="20"/>
+        <v>43.475306218592955</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="23"/>
+        <v>12.180760573701841</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>192</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.57</v>
+      </c>
+      <c r="D32" s="2">
+        <v>46.28</v>
+      </c>
+      <c r="E32" s="2">
+        <v>676.9</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="17"/>
+        <v>723.18</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1083.78</v>
+      </c>
+      <c r="H32" s="2">
+        <v>491.35</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="21"/>
+        <v>1083.78</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="22"/>
+        <v>1575.13</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" ref="K32" si="24">SUM(C32:H32)</f>
+        <v>3023.06</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="19"/>
+        <v>60.276587499307979</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="20"/>
+        <v>42.183299156260112</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="23"/>
+        <v>11.81877051417978</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2">
-        <v>4.59</v>
-      </c>
-      <c r="D25" s="2">
-        <v>89.4</v>
-      </c>
-      <c r="E25" s="2">
-        <v>609.38</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="15"/>
-        <v>698.78</v>
-      </c>
-      <c r="G25" s="2">
-        <v>9847.83</v>
-      </c>
-      <c r="H25" s="2">
-        <v>316.93</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="19"/>
-        <v>9847.83</v>
-      </c>
-      <c r="J25" s="2">
-        <f t="shared" si="20"/>
-        <v>10164.76</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="16"/>
-        <v>10868.13</v>
-      </c>
-      <c r="L25" s="2">
-        <f t="shared" si="17"/>
-        <v>6.633599483337953</v>
-      </c>
-      <c r="M25" s="2">
-        <f t="shared" si="18"/>
-        <v>6.5367190174681928</v>
+      <c r="K34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B26">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2">
+        <f>E35+D35</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2">
+        <f>G35</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <f>H35+G35</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <f>H35+G35+E35+D35+C35</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="e">
+        <f>$I$35/I35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="2" t="e">
+        <f>$J$35/J35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35">
+        <f>25000/3600</f>
+        <v>6.9444444444444446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2">
+        <f t="shared" ref="F36:F43" si="25">E36+D36</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2">
+        <f>G36</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <f>H36+G36</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" ref="K36:K42" si="26">H36+G36+E36+D36+C36</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="2" t="e">
+        <f t="shared" ref="L36:L43" si="27">$I$35/I36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36" s="2" t="e">
+        <f t="shared" ref="M36:M43" si="28">$J$35/J36</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1029.98</v>
+      </c>
+      <c r="E37" s="2">
+        <v>60.19</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="25"/>
+        <v>1090.17</v>
+      </c>
+      <c r="G37" s="2">
+        <v>101981.5</v>
+      </c>
+      <c r="H37" s="2">
+        <v>609.65</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" ref="I37:I43" si="29">G37</f>
+        <v>101981.5</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" ref="J37:J43" si="30">H37+G37</f>
+        <v>102591.15</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="26"/>
+        <v>103685.84</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <f>$J$37/J37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2">
+        <v>4.45</v>
+      </c>
+      <c r="D38" s="2">
+        <v>688.32</v>
+      </c>
+      <c r="E38" s="2">
+        <v>76.66</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="25"/>
+        <v>764.98</v>
+      </c>
+      <c r="G38" s="2">
+        <v>54552.514999999999</v>
+      </c>
+      <c r="H38" s="2">
+        <v>515.73</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="29"/>
+        <v>54552.514999999999</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="30"/>
+        <v>55068.245000000003</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="26"/>
+        <v>55837.675000000003</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" ref="N38:N43" si="31">$J$37/J38</f>
+        <v>1.8629820144077587</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B39">
         <v>16</v>
       </c>
-      <c r="C26" s="2">
-        <v>5.63</v>
-      </c>
-      <c r="D26" s="2">
-        <v>121.17</v>
-      </c>
-      <c r="E26" s="2">
-        <v>610.03</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="15"/>
-        <v>731.19999999999993</v>
-      </c>
-      <c r="G26" s="2">
-        <v>5489.39</v>
-      </c>
-      <c r="H26" s="2">
-        <v>309.16000000000003</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="19"/>
-        <v>5489.39</v>
-      </c>
-      <c r="J26" s="2">
-        <f t="shared" si="20"/>
-        <v>5798.55</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="16"/>
-        <v>6535.38</v>
-      </c>
-      <c r="L26" s="2">
-        <f t="shared" si="17"/>
-        <v>11.90051353611239</v>
-      </c>
-      <c r="M26" s="2">
-        <f t="shared" si="18"/>
-        <v>11.458757792896499</v>
+      <c r="C39" s="2">
+        <v>4.58</v>
+      </c>
+      <c r="D39" s="2">
+        <v>156.6</v>
+      </c>
+      <c r="E39" s="2">
+        <v>608.84</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="25"/>
+        <v>765.44</v>
+      </c>
+      <c r="G39" s="2">
+        <v>30366.98</v>
+      </c>
+      <c r="H39" s="2">
+        <v>371.24</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="29"/>
+        <v>30366.98</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="30"/>
+        <v>30738.22</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="26"/>
+        <v>31508.240000000002</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="31"/>
+        <v>3.3375761511239097</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B27">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B40">
         <v>32</v>
       </c>
-      <c r="C27" s="2">
-        <v>3.31</v>
-      </c>
-      <c r="D27" s="2">
-        <v>191.77</v>
-      </c>
-      <c r="E27" s="2">
-        <v>572.22</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" si="15"/>
-        <v>763.99</v>
-      </c>
-      <c r="G27" s="2">
-        <v>3196.4</v>
-      </c>
-      <c r="H27" s="2">
-        <v>220.92</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="19"/>
-        <v>3196.4</v>
-      </c>
-      <c r="J27" s="2">
-        <f t="shared" si="20"/>
-        <v>3417.32</v>
-      </c>
-      <c r="K27" s="2">
-        <f t="shared" si="16"/>
-        <v>4184.6200000000008</v>
-      </c>
-      <c r="L27" s="2">
-        <f t="shared" si="17"/>
-        <v>20.437542235014391</v>
-      </c>
-      <c r="M27" s="2">
-        <f t="shared" si="18"/>
-        <v>19.443359123523695</v>
+      <c r="C40" s="2">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="D40" s="2">
+        <v>215.26</v>
+      </c>
+      <c r="E40" s="2">
+        <v>597.63</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="25"/>
+        <v>812.89</v>
+      </c>
+      <c r="G40" s="2">
+        <v>17569.5</v>
+      </c>
+      <c r="H40" s="2">
+        <v>313.35000000000002</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="29"/>
+        <v>17569.5</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="30"/>
+        <v>17882.849999999999</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="26"/>
+        <v>18700.55</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="31"/>
+        <v>5.7368456370209451</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B41">
         <v>64</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>356.63</v>
-      </c>
-      <c r="E28" s="2">
-        <v>531.79</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="15"/>
-        <v>888.42</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1917.8</v>
-      </c>
-      <c r="H28" s="2">
-        <v>272.37</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="19"/>
-        <v>1917.8</v>
-      </c>
-      <c r="J28" s="2">
-        <f t="shared" si="20"/>
-        <v>2190.17</v>
-      </c>
-      <c r="K28" s="2">
-        <f t="shared" si="16"/>
-        <v>3079.59</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="17"/>
-        <v>34.063280842632182</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="18"/>
-        <v>30.337453257053102</v>
+      <c r="C41" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="D41" s="2">
+        <v>402.8</v>
+      </c>
+      <c r="E41" s="2">
+        <v>560.17999999999995</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="25"/>
+        <v>962.98</v>
+      </c>
+      <c r="G41" s="2">
+        <v>10321.89</v>
+      </c>
+      <c r="H41" s="2">
+        <v>309.33</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="29"/>
+        <v>10321.89</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="30"/>
+        <v>10631.22</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="26"/>
+        <v>11596.949999999999</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="31"/>
+        <v>9.6499884303024484</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B29">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B42">
         <v>128</v>
       </c>
-      <c r="C29" s="2">
-        <v>1.36</v>
-      </c>
-      <c r="D29" s="2">
-        <v>51.01</v>
-      </c>
-      <c r="E29" s="2">
-        <v>549.41999999999996</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="15"/>
-        <v>600.42999999999995</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1210.3800000000001</v>
-      </c>
-      <c r="H29" s="2">
-        <v>317.94</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="19"/>
-        <v>1210.3800000000001</v>
-      </c>
-      <c r="J29" s="2">
-        <f t="shared" si="20"/>
-        <v>1528.3200000000002</v>
-      </c>
-      <c r="K29" s="2">
-        <f t="shared" si="16"/>
-        <v>2130.1100000000006</v>
-      </c>
-      <c r="L29" s="2">
-        <f t="shared" si="17"/>
-        <v>53.971942695682344</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="18"/>
-        <v>43.475306218592955</v>
+      <c r="C42" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="D42" s="2">
+        <v>86.49</v>
+      </c>
+      <c r="E42" s="2">
+        <v>558.38</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="25"/>
+        <v>644.87</v>
+      </c>
+      <c r="G42" s="2">
+        <v>6139.34</v>
+      </c>
+      <c r="H42" s="2">
+        <v>356.76</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="29"/>
+        <v>6139.34</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="30"/>
+        <v>6496.1</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="26"/>
+        <v>7142.25</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="31"/>
+        <v>15.79272948384415</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B30">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B43">
         <v>192</v>
       </c>
-      <c r="C30" s="2">
-        <v>1.57</v>
-      </c>
-      <c r="D30" s="2">
-        <v>46.28</v>
-      </c>
-      <c r="E30" s="2">
-        <v>676.9</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="15"/>
-        <v>723.18</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1083.78</v>
-      </c>
-      <c r="H30" s="2">
-        <v>491.35</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="19"/>
-        <v>1083.78</v>
-      </c>
-      <c r="J30" s="2">
-        <f t="shared" si="20"/>
-        <v>1575.13</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" ref="K30" si="21">SUM(C30:H30)</f>
-        <v>3023.06</v>
-      </c>
-      <c r="L30" s="2">
-        <f t="shared" si="17"/>
-        <v>60.276587499307979</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="18"/>
-        <v>42.183299156260112</v>
+      <c r="C43" s="2">
+        <v>2.06</v>
+      </c>
+      <c r="D43" s="2">
+        <v>163.91</v>
+      </c>
+      <c r="E43" s="2">
+        <v>735.52</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="25"/>
+        <v>899.43</v>
+      </c>
+      <c r="G43" s="2">
+        <v>5033.28</v>
+      </c>
+      <c r="H43" s="2">
+        <v>716.92</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="29"/>
+        <v>5033.28</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="30"/>
+        <v>5750.2</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" ref="K43" si="32">SUM(C43:H43)</f>
+        <v>7551.12</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="31"/>
+        <v>17.841318562832598</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="1" t="s">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B45">
         <v>8</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>11</v>
+      <c r="K45">
+        <f>2*K46</f>
+        <v>25.768888888888888</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D33" s="2">
-        <v>2694.46</v>
-      </c>
-      <c r="E33" s="2">
-        <v>22.93</v>
-      </c>
-      <c r="F33" s="2">
-        <f>E33+D33</f>
-        <v>2717.39</v>
-      </c>
-      <c r="G33" s="2">
-        <v>41617.19</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1106.7</v>
-      </c>
-      <c r="I33" s="2">
-        <f>G33</f>
-        <v>41617.19</v>
-      </c>
-      <c r="J33" s="2">
-        <f>H33+G33</f>
-        <v>42723.89</v>
-      </c>
-      <c r="K33" s="2">
-        <f>H33+G33+E33+D33+C33</f>
-        <v>45445.38</v>
-      </c>
-      <c r="L33" s="2">
-        <f>$I$33/I33</f>
-        <v>1</v>
-      </c>
-      <c r="M33" s="2">
-        <f>$J$33/J33</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2">
-        <v>3.98</v>
-      </c>
-      <c r="D34" s="2">
-        <v>1337</v>
-      </c>
-      <c r="E34" s="2">
-        <v>388.16</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" ref="F34:F41" si="22">E34+D34</f>
-        <v>1725.16</v>
-      </c>
-      <c r="G34" s="2">
-        <v>21398.61</v>
-      </c>
-      <c r="H34" s="2">
-        <v>627.86</v>
-      </c>
-      <c r="I34" s="2">
-        <f>G34</f>
-        <v>21398.61</v>
-      </c>
-      <c r="J34" s="2">
-        <f>H34+G34</f>
-        <v>22026.47</v>
-      </c>
-      <c r="K34" s="2">
-        <f t="shared" ref="K34:K40" si="23">H34+G34+E34+D34+C34</f>
-        <v>23755.61</v>
-      </c>
-      <c r="L34" s="2">
-        <f t="shared" ref="L34:L41" si="24">$I$33/I34</f>
-        <v>1.9448548293557386</v>
-      </c>
-      <c r="M34" s="2">
-        <f t="shared" ref="M34:M41" si="25">$J$33/J34</f>
-        <v>1.9396612348687736</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35" s="2">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="D35" s="2">
-        <v>566.05999999999995</v>
-      </c>
-      <c r="E35" s="2">
-        <v>487.95</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="22"/>
-        <v>1054.01</v>
-      </c>
-      <c r="G35" s="2">
-        <v>11174.78</v>
-      </c>
-      <c r="H35" s="2">
-        <v>443.86</v>
-      </c>
-      <c r="I35" s="2">
-        <f t="shared" ref="I35:I41" si="26">G35</f>
-        <v>11174.78</v>
-      </c>
-      <c r="J35" s="2">
-        <f t="shared" ref="J35:J41" si="27">H35+G35</f>
-        <v>11618.640000000001</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" si="23"/>
-        <v>12677.04</v>
-      </c>
-      <c r="L35" s="2">
-        <f t="shared" si="24"/>
-        <v>3.724206651048164</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="25"/>
-        <v>3.6771851094448227</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2">
-        <v>87.74</v>
-      </c>
-      <c r="E36" s="2">
-        <v>598.04999999999995</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="22"/>
-        <v>685.79</v>
-      </c>
-      <c r="G36" s="2">
-        <v>5598.69</v>
-      </c>
-      <c r="H36" s="2">
-        <v>314.02</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="26"/>
-        <v>5598.69</v>
-      </c>
-      <c r="J36" s="2">
-        <f t="shared" si="27"/>
-        <v>5912.7099999999991</v>
-      </c>
-      <c r="K36" s="2">
-        <f t="shared" si="23"/>
-        <v>6602.4999999999991</v>
-      </c>
-      <c r="L36" s="2">
-        <f t="shared" si="24"/>
-        <v>7.4333799513814851</v>
-      </c>
-      <c r="M36" s="2">
-        <f t="shared" si="25"/>
-        <v>7.2257712622469237</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B46">
         <v>16</v>
       </c>
-      <c r="C37" s="2">
-        <v>5.63</v>
-      </c>
-      <c r="D37" s="2">
-        <v>124.82</v>
-      </c>
-      <c r="E37" s="2">
-        <v>596.51</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="22"/>
-        <v>721.32999999999993</v>
-      </c>
-      <c r="G37" s="2">
-        <v>2925.42</v>
-      </c>
-      <c r="H37" s="2">
-        <v>308.24</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="26"/>
-        <v>2925.42</v>
-      </c>
-      <c r="J37" s="2">
-        <f t="shared" si="27"/>
-        <v>3233.66</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="23"/>
-        <v>3960.6200000000003</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="24"/>
-        <v>14.226056429504141</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="25"/>
-        <v>13.212239382000583</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <v>32</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1.92</v>
-      </c>
-      <c r="D38" s="2">
-        <v>181.37</v>
-      </c>
-      <c r="E38" s="2">
-        <v>551.03</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="22"/>
-        <v>732.4</v>
-      </c>
-      <c r="G38" s="2">
-        <v>1561.23</v>
-      </c>
-      <c r="H38" s="2">
-        <v>220.92</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="26"/>
-        <v>1561.23</v>
-      </c>
-      <c r="J38" s="2">
-        <f t="shared" si="27"/>
-        <v>1782.15</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="23"/>
-        <v>2516.4700000000003</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="24"/>
-        <v>26.656668139864081</v>
-      </c>
-      <c r="M38" s="2">
-        <f t="shared" si="25"/>
-        <v>23.973228965014165</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B39">
-        <v>64</v>
-      </c>
-      <c r="C39" s="2">
-        <v>2.75</v>
-      </c>
-      <c r="D39" s="2">
-        <v>402.8</v>
-      </c>
-      <c r="E39" s="2">
-        <v>560.17999999999995</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="22"/>
-        <v>962.98</v>
-      </c>
-      <c r="G39" s="2">
-        <v>10321.89</v>
-      </c>
-      <c r="H39" s="2">
-        <v>309.33</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="26"/>
-        <v>10321.89</v>
-      </c>
-      <c r="J39" s="2">
-        <f t="shared" si="27"/>
-        <v>10631.22</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="23"/>
-        <v>11596.949999999999</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="24"/>
-        <v>4.0319350429039646</v>
-      </c>
-      <c r="M39" s="2">
-        <f t="shared" si="25"/>
-        <v>4.0187193943874737</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>128</v>
-      </c>
-      <c r="C40" s="2">
-        <v>1.06</v>
-      </c>
-      <c r="D40" s="2">
-        <v>61.5</v>
-      </c>
-      <c r="E40" s="2">
-        <v>530.94000000000005</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" si="22"/>
-        <v>592.44000000000005</v>
-      </c>
-      <c r="G40" s="2">
-        <v>565.16999999999996</v>
-      </c>
-      <c r="H40" s="2">
-        <v>277.91000000000003</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="26"/>
-        <v>565.16999999999996</v>
-      </c>
-      <c r="J40" s="2">
-        <f t="shared" si="27"/>
-        <v>843.07999999999993</v>
-      </c>
-      <c r="K40" s="2">
-        <f t="shared" si="23"/>
-        <v>1436.58</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="24"/>
-        <v>73.636587221543977</v>
-      </c>
-      <c r="M40" s="2">
-        <f t="shared" si="25"/>
-        <v>50.675961949043987</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <v>196</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1.68</v>
-      </c>
-      <c r="D41" s="2">
-        <v>48.21</v>
-      </c>
-      <c r="E41" s="2">
-        <v>587.71</v>
-      </c>
-      <c r="F41" s="2">
-        <f t="shared" si="22"/>
-        <v>635.92000000000007</v>
-      </c>
-      <c r="G41" s="2">
-        <v>499</v>
-      </c>
-      <c r="H41" s="2">
-        <v>352.78</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="26"/>
-        <v>499</v>
-      </c>
-      <c r="J41" s="2">
-        <f t="shared" si="27"/>
-        <v>851.78</v>
-      </c>
-      <c r="K41" s="2">
-        <f t="shared" ref="K41" si="28">SUM(C41:H41)</f>
-        <v>2125.3000000000002</v>
-      </c>
-      <c r="L41" s="2">
-        <f t="shared" si="24"/>
-        <v>83.401182364729465</v>
-      </c>
-      <c r="M41" s="2">
-        <f t="shared" si="25"/>
-        <v>50.158362487966379</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43">
-        <v>8</v>
-      </c>
-      <c r="K43">
-        <f>2*K44</f>
-        <v>25.768888888888888</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B44">
-        <v>16</v>
-      </c>
-      <c r="K44">
-        <f>2*K45</f>
+      <c r="K46">
+        <f>2*K47</f>
         <v>12.884444444444444</v>
       </c>
-      <c r="O44">
+      <c r="O46">
         <f>141/210</f>
         <v>0.67142857142857137</v>
       </c>
-      <c r="P44">
-        <f>O44*1917</f>
+      <c r="P46">
+        <f>O46*1917</f>
         <v>1287.1285714285714</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B45">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B47">
         <v>32</v>
       </c>
-      <c r="K45">
-        <f>2*K46</f>
+      <c r="K47">
+        <f>2*K48</f>
         <v>6.4422222222222221</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B46">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B48">
         <v>64</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K48" s="2">
         <f>11596/3600</f>
         <v>3.221111111111111</v>
       </c>
-      <c r="O46">
+      <c r="O48">
         <f>585/882</f>
         <v>0.66326530612244894</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B47">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49">
         <v>128</v>
       </c>
-      <c r="K47">
-        <f>0.5*K46</f>
+      <c r="K49">
+        <f>0.5*K48</f>
         <v>1.6105555555555555</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B48">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50">
         <v>192</v>
       </c>
-      <c r="K48">
-        <f>K47*128/192</f>
+      <c r="K50">
+        <f>K49*128/192</f>
         <v>1.0737037037037036</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Should be the same.
git-svn-id: svn://136.177.114.72/svn_GW/phast3/trunk@9602 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/src/phast/yeti.xlsx
+++ b/src/phast/yeti.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t>Easy 1D</t>
   </si>
@@ -101,6 +102,9 @@
   </si>
   <si>
     <t>seconds</t>
+  </si>
+  <si>
+    <t>Normalized chem w messages</t>
   </si>
 </sst>
 </file>
@@ -529,7 +533,7 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="256"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2652,16 +2656,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
+      <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2682,16 +2686,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2980,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2991,6 +2995,7 @@
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.77734375" customWidth="1"/>
     <col min="10" max="12" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -3004,7 +3009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3043,6 +3048,9 @@
       </c>
       <c r="M2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3088,6 +3096,10 @@
         <f>$J$3/J3</f>
         <v>1</v>
       </c>
+      <c r="O3">
+        <f>J3/8.81</f>
+        <v>4849.4767309875142</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -3131,6 +3143,10 @@
       <c r="M4" s="2">
         <f>$J$3/J4</f>
         <v>1.9396612348687736</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O11" si="2">J4/8.81</f>
+        <v>2500.1668558456299</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -3161,11 +3177,11 @@
         <v>443.86</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I11" si="2">G5</f>
+        <f t="shared" ref="I5:I11" si="3">G5</f>
         <v>11174.78</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J11" si="3">H5+G5</f>
+        <f t="shared" ref="J5:J11" si="4">H5+G5</f>
         <v>11618.640000000001</v>
       </c>
       <c r="K5" s="2">
@@ -3173,21 +3189,25 @@
         <v>12677.04</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L11" si="4">$I$3/I5</f>
+        <f t="shared" ref="L5:L11" si="5">$I$3/I5</f>
         <v>3.724206651048164</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M10" si="5">$J$3/J5</f>
+        <f t="shared" ref="M5:M10" si="6">$J$3/J5</f>
         <v>3.6771851094448227</v>
       </c>
       <c r="N5" s="2">
         <f>$J$5/J5</f>
         <v>1</v>
       </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>1318.8013620885358</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A11" si="6">B6/$B$5</f>
+        <f t="shared" ref="A6:A11" si="7">B6/$B$5</f>
         <v>2</v>
       </c>
       <c r="B6">
@@ -3213,11 +3233,11 @@
         <v>314.02</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5598.69</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5912.7099999999991</v>
       </c>
       <c r="K6" s="2">
@@ -3225,21 +3245,25 @@
         <v>6602.4999999999991</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.4333799513814851</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.2257712622469237</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" ref="N6:N11" si="7">$J$5/J6</f>
+        <f t="shared" ref="N6:N11" si="8">$J$5/J6</f>
         <v>1.9650278806165029</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>671.13620885357534</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B7">
@@ -3265,11 +3289,11 @@
         <v>308.24</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2925.42</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3233.66</v>
       </c>
       <c r="K7" s="2">
@@ -3277,21 +3301,25 @@
         <v>3960.6200000000003</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.226056429504141</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13.212239382000583</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.5930308071967993</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>367.04426787741198</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B8">
@@ -3317,11 +3345,11 @@
         <v>220.92</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1561.23</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1782.15</v>
       </c>
       <c r="K8" s="2">
@@ -3329,21 +3357,25 @@
         <v>2516.4700000000003</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.656668139864081</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23.973228965014165</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.5194512246443903</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>202.28717366628831</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="B9">
@@ -3369,11 +3401,11 @@
         <v>262.8</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1032.0999999999999</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1294.8999999999999</v>
       </c>
       <c r="K9" s="2">
@@ -3381,21 +3413,25 @@
         <v>2173.7199999999998</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.322827245421962</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32.993968646227508</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.9726156459958322</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>146.98070374574345</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="B10">
@@ -3421,11 +3457,11 @@
         <v>277.91000000000003</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>565.16999999999996</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>843.07999999999993</v>
       </c>
       <c r="K10" s="2">
@@ -3433,21 +3469,25 @@
         <v>1436.58</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.636587221543977</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50.675961949043987</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13.781183280352995</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>95.695800227014743</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="B11">
@@ -3463,7 +3503,7 @@
         <v>587.71</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" ref="F11" si="8">E11+D11</f>
+        <f t="shared" ref="F11" si="9">E11+D11</f>
         <v>635.92000000000007</v>
       </c>
       <c r="G11" s="2">
@@ -3473,19 +3513,19 @@
         <v>352.78</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>499</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>851.78</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" ref="K11" si="9">SUM(C11:H11)</f>
+        <f t="shared" ref="K11" si="10">SUM(C11:H11)</f>
         <v>2125.3000000000002</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83.401182364729465</v>
       </c>
       <c r="M11" s="2">
@@ -3493,8 +3533,12 @@
         <v>50.158362487966379</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13.640423583554441</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>96.683314415436996</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -3562,7 +3606,7 @@
         <v>1108</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" ref="I14:I21" si="10">G14</f>
+        <f t="shared" ref="I14:I21" si="11">G14</f>
         <v>41304.5</v>
       </c>
       <c r="J14" s="2">
@@ -3580,6 +3624,10 @@
       <c r="M14" s="2">
         <f>$J$14/J14</f>
         <v>1</v>
+      </c>
+      <c r="O14">
+        <f>J14/8.81</f>
+        <v>4814.1316685584561</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -3596,7 +3644,7 @@
         <v>17.63</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" ref="F15:F21" si="11">E15+D15</f>
+        <f t="shared" ref="F15:F21" si="12">E15+D15</f>
         <v>2417.2600000000002</v>
       </c>
       <c r="G15" s="2">
@@ -3606,7 +3654,7 @@
         <v>845.38</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21521.13</v>
       </c>
       <c r="J15" s="2">
@@ -3622,8 +3670,12 @@
         <v>1.9337827521138529</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ref="M15:M18" si="12">$J$3/J15</f>
+        <f t="shared" ref="M15:M18" si="13">$J$3/J15</f>
         <v>1.9101723961404795</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15:O21" si="14">J15/8.81</f>
+        <v>2538.7639046538025</v>
       </c>
       <c r="P15" s="3"/>
     </row>
@@ -3641,7 +3693,7 @@
         <v>19.63</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1553.0100000000002</v>
       </c>
       <c r="G16" s="2">
@@ -3651,28 +3703,32 @@
         <v>758.5</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10877.25</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" ref="J16:J21" si="13">H16+G16</f>
+        <f t="shared" ref="J16:J21" si="15">H16+G16</f>
         <v>11635.75</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" ref="K16:K17" si="14">SUM(C16:H16)</f>
+        <f t="shared" ref="K16:K17" si="16">SUM(C16:H16)</f>
         <v>14743.27</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" ref="L16:L17" si="15">$I$3/I16</f>
+        <f t="shared" ref="L16:L17" si="17">$I$3/I16</f>
         <v>3.8260764439541246</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.6717779257890553</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="14"/>
+        <v>1320.743473325766</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>8</v>
       </c>
@@ -3686,7 +3742,7 @@
         <v>67.63</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2044.0100000000002</v>
       </c>
       <c r="G17" s="2">
@@ -3696,27 +3752,31 @@
         <v>961.88</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5946.63</v>
       </c>
       <c r="J17" s="2">
+        <f t="shared" si="15"/>
+        <v>6908.51</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="16"/>
+        <v>11005.28</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="17"/>
+        <v>6.9984495420095083</v>
+      </c>
+      <c r="M17" s="2">
         <f t="shared" si="13"/>
-        <v>6908.51</v>
-      </c>
-      <c r="K17" s="2">
+        <v>6.1842408855165587</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="14"/>
-        <v>11005.28</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="15"/>
-        <v>6.9984495420095083</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="12"/>
-        <v>6.1842408855165587</v>
+        <v>784.16685584562993</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -3730,7 +3790,7 @@
         <v>33.22</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1459.8500000000001</v>
       </c>
       <c r="G18" s="2">
@@ -3740,11 +3800,11 @@
         <v>1699.91</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3442.97</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5142.88</v>
       </c>
       <c r="K18" s="2">
@@ -3756,11 +3816,15 @@
         <v>12.087584265909957</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.3073861338394046</v>
       </c>
+      <c r="O18">
+        <f t="shared" si="14"/>
+        <v>583.75482406356412</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
@@ -3774,7 +3838,7 @@
         <v>33.380000000000003</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6571.76</v>
       </c>
       <c r="G19" s="2">
@@ -3784,11 +3848,11 @@
         <v>8057.44</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11432</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>19489.439999999999</v>
       </c>
       <c r="K19" s="2">
@@ -3800,11 +3864,15 @@
         <v>3.6404120013995804</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" ref="M19:M21" si="16">$J$3/J19</f>
+        <f t="shared" ref="M19:M21" si="18">$J$3/J19</f>
         <v>2.192155854657702</v>
       </c>
+      <c r="O19">
+        <f t="shared" si="14"/>
+        <v>2212.1952326901246</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>32</v>
       </c>
@@ -3818,7 +3886,7 @@
         <v>43.13</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6730.88</v>
       </c>
       <c r="G20" s="2">
@@ -3828,11 +3896,11 @@
         <v>8750.75</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7414.25</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>16165</v>
       </c>
       <c r="K20" s="2">
@@ -3844,11 +3912,15 @@
         <v>5.6131355160670333</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.6429873182802353</v>
       </c>
+      <c r="O20">
+        <f t="shared" si="14"/>
+        <v>1834.8467650397274</v>
+      </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>64</v>
       </c>
@@ -3862,7 +3934,7 @@
         <v>105.63</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10779.509999999998</v>
       </c>
       <c r="G21" s="2">
@@ -3872,11 +3944,11 @@
         <v>20880.88</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11745.56</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>32626.440000000002</v>
       </c>
       <c r="K21" s="2">
@@ -3888,11 +3960,15 @@
         <v>3.5432273982679416</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.3094867230381249</v>
       </c>
+      <c r="O21">
+        <f t="shared" si="14"/>
+        <v>3703.3416572077185</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -3905,7 +3981,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -3946,7 +4022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -3990,7 +4066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>2</v>
       </c>
@@ -4004,7 +4080,7 @@
         <v>349.21</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" ref="F25:F32" si="17">E25+D25</f>
+        <f t="shared" ref="F25:F32" si="19">E25+D25</f>
         <v>1665.82</v>
       </c>
       <c r="G25" s="2">
@@ -4022,19 +4098,19 @@
         <v>34700.57</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" ref="K25:K31" si="18">H25+G25+E25+D25+C25</f>
+        <f t="shared" ref="K25:K31" si="20">H25+G25+E25+D25+C25</f>
         <v>36370.879999999997</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" ref="L25:L32" si="19">$I$24/I25</f>
+        <f t="shared" ref="L25:L32" si="21">$I$24/I25</f>
         <v>1.9199655781096527</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" ref="M25:M32" si="20">$J$24/J25</f>
+        <f t="shared" ref="M25:M32" si="22">$J$24/J25</f>
         <v>1.9147864141712945</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>4</v>
       </c>
@@ -4048,7 +4124,7 @@
         <v>476.04</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1029.3499999999999</v>
       </c>
       <c r="G26" s="2">
@@ -4058,23 +4134,23 @@
         <v>494.96</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26:I32" si="21">G26</f>
+        <f t="shared" ref="I26:I32" si="23">G26</f>
         <v>18121.14</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" ref="J26:J32" si="22">H26+G26</f>
+        <f t="shared" ref="J26:J32" si="24">H26+G26</f>
         <v>18616.099999999999</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>19650.010000000002</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.6049917389303321</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.5691782919086168</v>
       </c>
       <c r="N26" s="2">
@@ -4082,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>8</v>
       </c>
@@ -4096,7 +4172,7 @@
         <v>609.38</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>698.78</v>
       </c>
       <c r="G27" s="2">
@@ -4106,31 +4182,31 @@
         <v>316.93</v>
       </c>
       <c r="I27" s="2">
+        <f t="shared" si="23"/>
+        <v>9847.83</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="24"/>
+        <v>10164.76</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="20"/>
+        <v>10868.13</v>
+      </c>
+      <c r="L27" s="2">
         <f t="shared" si="21"/>
-        <v>9847.83</v>
-      </c>
-      <c r="J27" s="2">
+        <v>6.633599483337953</v>
+      </c>
+      <c r="M27" s="2">
         <f t="shared" si="22"/>
-        <v>10164.76</v>
-      </c>
-      <c r="K27" s="2">
-        <f t="shared" si="18"/>
-        <v>10868.13</v>
-      </c>
-      <c r="L27" s="2">
-        <f t="shared" si="19"/>
-        <v>6.633599483337953</v>
-      </c>
-      <c r="M27" s="2">
-        <f t="shared" si="20"/>
         <v>6.5367190174681928</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N32" si="23">$J$26/J27</f>
+        <f t="shared" ref="N27:N32" si="25">$J$26/J27</f>
         <v>1.8314352724510956</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>16</v>
       </c>
@@ -4144,7 +4220,7 @@
         <v>610.03</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>731.19999999999993</v>
       </c>
       <c r="G28" s="2">
@@ -4154,31 +4230,31 @@
         <v>309.16000000000003</v>
       </c>
       <c r="I28" s="2">
+        <f t="shared" si="23"/>
+        <v>5489.39</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="24"/>
+        <v>5798.55</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="20"/>
+        <v>6535.38</v>
+      </c>
+      <c r="L28" s="2">
         <f t="shared" si="21"/>
-        <v>5489.39</v>
-      </c>
-      <c r="J28" s="2">
+        <v>11.90051353611239</v>
+      </c>
+      <c r="M28" s="2">
         <f t="shared" si="22"/>
-        <v>5798.55</v>
-      </c>
-      <c r="K28" s="2">
-        <f t="shared" si="18"/>
-        <v>6535.38</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="19"/>
-        <v>11.90051353611239</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="20"/>
         <v>11.458757792896499</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>3.210475032551241</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>32</v>
       </c>
@@ -4192,7 +4268,7 @@
         <v>572.22</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>763.99</v>
       </c>
       <c r="G29" s="2">
@@ -4202,31 +4278,31 @@
         <v>220.92</v>
       </c>
       <c r="I29" s="2">
+        <f t="shared" si="23"/>
+        <v>3196.4</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="24"/>
+        <v>3417.32</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="20"/>
+        <v>4184.6200000000008</v>
+      </c>
+      <c r="L29" s="2">
         <f t="shared" si="21"/>
-        <v>3196.4</v>
-      </c>
-      <c r="J29" s="2">
+        <v>20.437542235014391</v>
+      </c>
+      <c r="M29" s="2">
         <f t="shared" si="22"/>
-        <v>3417.32</v>
-      </c>
-      <c r="K29" s="2">
-        <f t="shared" si="18"/>
-        <v>4184.6200000000008</v>
-      </c>
-      <c r="L29" s="2">
-        <f t="shared" si="19"/>
-        <v>20.437542235014391</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="20"/>
         <v>19.443359123523695</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.4475729519038305</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>64</v>
       </c>
@@ -4240,7 +4316,7 @@
         <v>531.79</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>888.42</v>
       </c>
       <c r="G30" s="2">
@@ -4250,31 +4326,31 @@
         <v>272.37</v>
       </c>
       <c r="I30" s="2">
+        <f t="shared" si="23"/>
+        <v>1917.8</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="24"/>
+        <v>2190.17</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="20"/>
+        <v>3079.59</v>
+      </c>
+      <c r="L30" s="2">
         <f t="shared" si="21"/>
-        <v>1917.8</v>
-      </c>
-      <c r="J30" s="2">
+        <v>34.063280842632182</v>
+      </c>
+      <c r="M30" s="2">
         <f t="shared" si="22"/>
-        <v>2190.17</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" si="18"/>
-        <v>3079.59</v>
-      </c>
-      <c r="L30" s="2">
-        <f t="shared" si="19"/>
-        <v>34.063280842632182</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="20"/>
         <v>30.337453257053102</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>8.4998424779811597</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>128</v>
       </c>
@@ -4288,7 +4364,7 @@
         <v>549.41999999999996</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>600.42999999999995</v>
       </c>
       <c r="G31" s="2">
@@ -4298,31 +4374,31 @@
         <v>317.94</v>
       </c>
       <c r="I31" s="2">
+        <f t="shared" si="23"/>
+        <v>1210.3800000000001</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="24"/>
+        <v>1528.3200000000002</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="20"/>
+        <v>2130.1100000000006</v>
+      </c>
+      <c r="L31" s="2">
         <f t="shared" si="21"/>
-        <v>1210.3800000000001</v>
-      </c>
-      <c r="J31" s="2">
+        <v>53.971942695682344</v>
+      </c>
+      <c r="M31" s="2">
         <f t="shared" si="22"/>
-        <v>1528.3200000000002</v>
-      </c>
-      <c r="K31" s="2">
-        <f t="shared" si="18"/>
-        <v>2130.1100000000006</v>
-      </c>
-      <c r="L31" s="2">
-        <f t="shared" si="19"/>
-        <v>53.971942695682344</v>
-      </c>
-      <c r="M31" s="2">
-        <f t="shared" si="20"/>
         <v>43.475306218592955</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>12.180760573701841</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>192</v>
       </c>
@@ -4336,7 +4412,7 @@
         <v>676.9</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>723.18</v>
       </c>
       <c r="G32" s="2">
@@ -4346,27 +4422,27 @@
         <v>491.35</v>
       </c>
       <c r="I32" s="2">
+        <f t="shared" si="23"/>
+        <v>1083.78</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="24"/>
+        <v>1575.13</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" ref="K32" si="26">SUM(C32:H32)</f>
+        <v>3023.06</v>
+      </c>
+      <c r="L32" s="2">
         <f t="shared" si="21"/>
-        <v>1083.78</v>
-      </c>
-      <c r="J32" s="2">
+        <v>60.276587499307979</v>
+      </c>
+      <c r="M32" s="2">
         <f t="shared" si="22"/>
-        <v>1575.13</v>
-      </c>
-      <c r="K32" s="2">
-        <f t="shared" ref="K32" si="24">SUM(C32:H32)</f>
-        <v>3023.06</v>
-      </c>
-      <c r="L32" s="2">
-        <f t="shared" si="19"/>
-        <v>60.276587499307979</v>
-      </c>
-      <c r="M32" s="2">
-        <f t="shared" si="20"/>
         <v>42.183299156260112</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11.81877051417978</v>
       </c>
     </row>
@@ -4457,7 +4533,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
-        <f t="shared" ref="F36:F43" si="25">E36+D36</f>
+        <f t="shared" ref="F36:F43" si="27">E36+D36</f>
         <v>0</v>
       </c>
       <c r="G36" s="2"/>
@@ -4471,15 +4547,15 @@
         <v>0</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" ref="K36:K42" si="26">H36+G36+E36+D36+C36</f>
+        <f t="shared" ref="K36:K42" si="28">H36+G36+E36+D36+C36</f>
         <v>0</v>
       </c>
       <c r="L36" s="2" t="e">
-        <f t="shared" ref="L36:L43" si="27">$I$35/I36</f>
+        <f t="shared" ref="L36:L43" si="29">$I$35/I36</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M36" s="2" t="e">
-        <f t="shared" ref="M36:M43" si="28">$J$35/J36</f>
+        <f t="shared" ref="M36:M43" si="30">$J$35/J36</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4497,7 +4573,7 @@
         <v>60.19</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>1090.17</v>
       </c>
       <c r="G37" s="2">
@@ -4507,23 +4583,23 @@
         <v>609.65</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" ref="I37:I43" si="29">G37</f>
+        <f t="shared" ref="I37:I43" si="31">G37</f>
         <v>101981.5</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" ref="J37:J43" si="30">H37+G37</f>
+        <f t="shared" ref="J37:J43" si="32">H37+G37</f>
         <v>102591.15</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>103685.84</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N37" s="2">
@@ -4545,7 +4621,7 @@
         <v>76.66</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>764.98</v>
       </c>
       <c r="G38" s="2">
@@ -4555,27 +4631,27 @@
         <v>515.73</v>
       </c>
       <c r="I38" s="2">
+        <f t="shared" si="31"/>
+        <v>54552.514999999999</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="32"/>
+        <v>55068.245000000003</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="28"/>
+        <v>55837.675000000003</v>
+      </c>
+      <c r="L38" s="2">
         <f t="shared" si="29"/>
-        <v>54552.514999999999</v>
-      </c>
-      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
         <f t="shared" si="30"/>
-        <v>55068.245000000003</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="26"/>
-        <v>55837.675000000003</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M38" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N38" s="2">
-        <f t="shared" ref="N38:N43" si="31">$J$37/J38</f>
+        <f t="shared" ref="N38:N43" si="33">$J$37/J38</f>
         <v>1.8629820144077587</v>
       </c>
     </row>
@@ -4593,7 +4669,7 @@
         <v>608.84</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>765.44</v>
       </c>
       <c r="G39" s="2">
@@ -4603,27 +4679,27 @@
         <v>371.24</v>
       </c>
       <c r="I39" s="2">
+        <f t="shared" si="31"/>
+        <v>30366.98</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="32"/>
+        <v>30738.22</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="28"/>
+        <v>31508.240000000002</v>
+      </c>
+      <c r="L39" s="2">
         <f t="shared" si="29"/>
-        <v>30366.98</v>
-      </c>
-      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
         <f t="shared" si="30"/>
-        <v>30738.22</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="26"/>
-        <v>31508.240000000002</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M39" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N39" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>3.3375761511239097</v>
       </c>
     </row>
@@ -4641,7 +4717,7 @@
         <v>597.63</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>812.89</v>
       </c>
       <c r="G40" s="2">
@@ -4651,27 +4727,27 @@
         <v>313.35000000000002</v>
       </c>
       <c r="I40" s="2">
+        <f t="shared" si="31"/>
+        <v>17569.5</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="32"/>
+        <v>17882.849999999999</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="28"/>
+        <v>18700.55</v>
+      </c>
+      <c r="L40" s="2">
         <f t="shared" si="29"/>
-        <v>17569.5</v>
-      </c>
-      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
         <f t="shared" si="30"/>
-        <v>17882.849999999999</v>
-      </c>
-      <c r="K40" s="2">
-        <f t="shared" si="26"/>
-        <v>18700.55</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M40" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5.7368456370209451</v>
       </c>
     </row>
@@ -4689,7 +4765,7 @@
         <v>560.17999999999995</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>962.98</v>
       </c>
       <c r="G41" s="2">
@@ -4699,27 +4775,27 @@
         <v>309.33</v>
       </c>
       <c r="I41" s="2">
+        <f t="shared" si="31"/>
+        <v>10321.89</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="32"/>
+        <v>10631.22</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="28"/>
+        <v>11596.949999999999</v>
+      </c>
+      <c r="L41" s="2">
         <f t="shared" si="29"/>
-        <v>10321.89</v>
-      </c>
-      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
         <f t="shared" si="30"/>
-        <v>10631.22</v>
-      </c>
-      <c r="K41" s="2">
-        <f t="shared" si="26"/>
-        <v>11596.949999999999</v>
-      </c>
-      <c r="L41" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M41" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N41" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>9.6499884303024484</v>
       </c>
     </row>
@@ -4737,7 +4813,7 @@
         <v>558.38</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>644.87</v>
       </c>
       <c r="G42" s="2">
@@ -4747,27 +4823,27 @@
         <v>356.76</v>
       </c>
       <c r="I42" s="2">
+        <f t="shared" si="31"/>
+        <v>6139.34</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="32"/>
+        <v>6496.1</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="28"/>
+        <v>7142.25</v>
+      </c>
+      <c r="L42" s="2">
         <f t="shared" si="29"/>
-        <v>6139.34</v>
-      </c>
-      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
         <f t="shared" si="30"/>
-        <v>6496.1</v>
-      </c>
-      <c r="K42" s="2">
-        <f t="shared" si="26"/>
-        <v>7142.25</v>
-      </c>
-      <c r="L42" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M42" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N42" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>15.79272948384415</v>
       </c>
     </row>
@@ -4785,7 +4861,7 @@
         <v>735.52</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>899.43</v>
       </c>
       <c r="G43" s="2">
@@ -4795,27 +4871,27 @@
         <v>716.92</v>
       </c>
       <c r="I43" s="2">
+        <f t="shared" si="31"/>
+        <v>5033.28</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="32"/>
+        <v>5750.2</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" ref="K43" si="34">SUM(C43:H43)</f>
+        <v>7551.12</v>
+      </c>
+      <c r="L43" s="2">
         <f t="shared" si="29"/>
-        <v>5033.28</v>
-      </c>
-      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
         <f t="shared" si="30"/>
-        <v>5750.2</v>
-      </c>
-      <c r="K43" s="2">
-        <f t="shared" ref="K43" si="32">SUM(C43:H43)</f>
-        <v>7551.12</v>
-      </c>
-      <c r="L43" s="2">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M43" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="N43" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>17.841318562832598</v>
       </c>
     </row>
@@ -4893,4 +4969,45 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H22:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <f>0.1*1*2</f>
+        <v>0.2</v>
+      </c>
+      <c r="I22">
+        <f>LOG10(H22)</f>
+        <v>-0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <f>0.1*10*2</f>
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <f>LOG10(H23)</f>
+        <v>0.3010299956639812</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f>1760/192</f>
+        <v>9.1666666666666661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>